<commit_message>
Day1 code some changes in terms of ChromeOptions and removing Thread.sleep
</commit_message>
<xml_diff>
--- a/src/test/java/com/rediff/qa/testData/RediffTestData.xlsx
+++ b/src/test/java/com/rediff/qa/testData/RediffTestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\autom\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{775FA168-08DB-4B32-A080-7AC1373D2A28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7A8B1DE-34A6-4790-9BD7-844E88EBFB03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>username</t>
   </si>
@@ -39,9 +39,6 @@
     <t>seleniumpanda1@rediffmail.com</t>
   </si>
   <si>
-    <t>seleniumpanda2@rediffmail.com</t>
-  </si>
-  <si>
     <t>Mohamedboudguig@rediffmail.com</t>
   </si>
   <si>
@@ -52,6 +49,18 @@
   </si>
   <si>
     <t>Medbdg0707@</t>
+  </si>
+  <si>
+    <t>jsmith2024@rediffmail.com</t>
+  </si>
+  <si>
+    <t>redcow@1999</t>
+  </si>
+  <si>
+    <t>homa_rahimi@rediffmail.com</t>
+  </si>
+  <si>
+    <t>Winter2021?</t>
   </si>
 </sst>
 </file>
@@ -117,11 +126,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -403,10 +413,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -428,7 +438,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -436,23 +446,31 @@
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -463,7 +481,9 @@
     <hyperlink ref="B2" r:id="rId4" xr:uid="{B9019B31-584F-49CC-BFFF-BB032F1E9A72}"/>
     <hyperlink ref="B3" r:id="rId5" xr:uid="{49BA3207-3EC6-461A-9400-B9FCB5788E70}"/>
     <hyperlink ref="B4" r:id="rId6" xr:uid="{55D3BBDF-ED9B-48B6-8328-03A9B4BFD1A9}"/>
+    <hyperlink ref="A6" r:id="rId7" xr:uid="{B69D97C4-5A6F-4B14-9C68-0171E1ECCDFA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
final code of Hybrid Framework for Rediff
</commit_message>
<xml_diff>
--- a/src/test/java/com/rediff/qa/testData/RediffTestData.xlsx
+++ b/src/test/java/com/rediff/qa/testData/RediffTestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\autom\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7A8B1DE-34A6-4790-9BD7-844E88EBFB03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6A7E8EC-1FA5-4606-B1B6-A274E2E0E018}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -51,23 +51,23 @@
     <t>Medbdg0707@</t>
   </si>
   <si>
-    <t>jsmith2024@rediffmail.com</t>
-  </si>
-  <si>
-    <t>redcow@1999</t>
-  </si>
-  <si>
     <t>homa_rahimi@rediffmail.com</t>
   </si>
   <si>
     <t>Winter2021?</t>
+  </si>
+  <si>
+    <t>Shajlee1@</t>
+  </si>
+  <si>
+    <t>chowdhurygs@rediffmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -78,6 +78,21 @@
     <font>
       <u/>
       <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="36"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="36"/>
       <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -126,12 +141,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -416,16 +432,15 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="115.140625" defaultRowHeight="46.5" x14ac:dyDescent="0.7"/>
   <cols>
-    <col min="1" max="1" width="34.28515625" customWidth="1"/>
-    <col min="2" max="2" width="36.28515625" customWidth="1"/>
+    <col min="1" max="16384" width="115.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -433,44 +448,44 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.7">
+      <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.7">
+      <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.7">
+      <c r="A4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.7">
+      <c r="A5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.7">
+      <c r="A6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B6" s="2" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>